<commit_message>
test data add references
</commit_message>
<xml_diff>
--- a/testData/test data.xlsx
+++ b/testData/test data.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jammytan/Documents/STV-Project/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C5AAC4-DB01-B340-8175-97FA71F02A77}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CB94CF5-AD62-2148-B8B6-41083FA80A23}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14220" xr2:uid="{0FD658B9-5079-5842-BC6B-31727AF6850F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1" xr2:uid="{0FD658B9-5079-5842-BC6B-31727AF6850F}"/>
   </bookViews>
   <sheets>
-    <sheet name="All" sheetId="1" r:id="rId1"/>
-    <sheet name="Home" sheetId="4" r:id="rId2"/>
-    <sheet name="CreateTasks_x0009_" sheetId="3" r:id="rId3"/>
-    <sheet name="ReviewTask" sheetId="7" r:id="rId4"/>
-    <sheet name="DisplayedLists" sheetId="9" r:id="rId5"/>
+    <sheet name="TaskList" sheetId="4" r:id="rId1"/>
+    <sheet name="EditTasks_x0009_" sheetId="3" r:id="rId2"/>
+    <sheet name="ViewTask" sheetId="7" r:id="rId3"/>
+    <sheet name="DisplayedLists" sheetId="9" r:id="rId4"/>
+    <sheet name="All" sheetId="1" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">ReviewTask!$A$1:$A$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">ViewTask!$A$1:$A$10</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="358">
   <si>
     <t>component</t>
   </si>
@@ -1306,15 +1306,9 @@
     <t>search_editText</t>
   </si>
   <si>
-    <t>search_close_btn</t>
-  </si>
-  <si>
     <t>//*[@resource-id='org.dmfs.tasks:id/search_close_btn']</t>
   </si>
   <si>
-    <t>delete_record_btn</t>
-  </si>
-  <si>
     <t>quick add</t>
   </si>
   <si>
@@ -1348,18 +1342,6 @@
     <t>menu</t>
   </si>
   <si>
-    <t>menu_displayed_lists</t>
-  </si>
-  <si>
-    <t>menu_settings</t>
-  </si>
-  <si>
-    <t>menu_show_completed_tasks</t>
-  </si>
-  <si>
-    <t>menu_refresh</t>
-  </si>
-  <si>
     <t>confirm delete</t>
   </si>
   <si>
@@ -1367,13 +1349,151 @@
   </si>
   <si>
     <t>color setting</t>
+  </si>
+  <si>
+    <t>status_dropdown</t>
+  </si>
+  <si>
+    <t>TaskList1.png</t>
+  </si>
+  <si>
+    <t>reference</t>
+  </si>
+  <si>
+    <t>QuickAdd.png</t>
+  </si>
+  <si>
+    <t>ConfirmDelete.png</t>
+  </si>
+  <si>
+    <t>TaskListMenu.png</t>
+  </si>
+  <si>
+    <t>TasksDue.png</t>
+  </si>
+  <si>
+    <t>TasksStarting.png</t>
+  </si>
+  <si>
+    <t>TasksPriority.png</t>
+  </si>
+  <si>
+    <t>TaskProgress.png</t>
+  </si>
+  <si>
+    <t>remove_record_btn</t>
+  </si>
+  <si>
+    <t>search_back_btn</t>
+  </si>
+  <si>
+    <t>Search.png</t>
+  </si>
+  <si>
+    <t>priority_dropdown</t>
+  </si>
+  <si>
+    <t>privacy_dropdown</t>
+  </si>
+  <si>
+    <t>time_zone_dropdown</t>
+  </si>
+  <si>
+    <t>EditTask1.png</t>
+  </si>
+  <si>
+    <t>folder_dropdown</t>
+  </si>
+  <si>
+    <t>FolderOptions.png</t>
+  </si>
+  <si>
+    <t>needs_action</t>
+  </si>
+  <si>
+    <t>in_process</t>
+  </si>
+  <si>
+    <t>cancelled</t>
+  </si>
+  <si>
+    <t>StatusOptions.png</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>not_specified</t>
+  </si>
+  <si>
+    <t>public</t>
+  </si>
+  <si>
+    <t>private</t>
+  </si>
+  <si>
+    <t>confidential</t>
+  </si>
+  <si>
+    <t>AM</t>
+  </si>
+  <si>
+    <t>PM</t>
+  </si>
+  <si>
+    <t>displayed_lists</t>
+  </si>
+  <si>
+    <t>settings</t>
+  </si>
+  <si>
+    <t>show_completed_tasks</t>
+  </si>
+  <si>
+    <t>refresh</t>
+  </si>
+  <si>
+    <t>EditTask2.png</t>
+  </si>
+  <si>
+    <t>previous_month</t>
+  </si>
+  <si>
+    <t>next_month</t>
+  </si>
+  <si>
+    <t>year_picker</t>
+  </si>
+  <si>
+    <t>date_picker</t>
+  </si>
+  <si>
+    <t>pick_date</t>
+  </si>
+  <si>
+    <t>pick_year</t>
+  </si>
+  <si>
+    <t>Calendar.png</t>
+  </si>
+  <si>
+    <t>CalendarPickYear.png</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1440,6 +1560,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1449,7 +1577,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -1509,11 +1637,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1581,8 +1728,43 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1894,10 +2076,1816 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EF6FCC3-78DA-E74D-BF53-4A0FCE774DC3}">
+  <dimension ref="A1:E60"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
+  <cols>
+    <col min="1" max="1" width="31" style="11" customWidth="1"/>
+    <col min="2" max="2" width="99.33203125" style="11" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" style="11" customWidth="1"/>
+    <col min="4" max="4" width="16.5" style="11" customWidth="1"/>
+    <col min="5" max="5" width="17.5" style="11" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="21" customHeight="1">
+      <c r="A1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>299</v>
+      </c>
+      <c r="E1" s="34" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" s="35" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="33"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" s="33"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="12"/>
+      <c r="E5" s="33"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="12"/>
+      <c r="E6" s="33"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="12"/>
+      <c r="E7" s="33"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="12"/>
+      <c r="E8" s="33"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="11" t="s">
+        <v>302</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="12"/>
+      <c r="E9" s="33"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E10" s="33"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="E11" s="33"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E12" s="36"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="28" t="s">
+        <v>298</v>
+      </c>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="30"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="E14" s="40" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="E15" s="40"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="E16" s="40"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="E17" s="40"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18" s="40"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="E19" s="40"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="28" t="s">
+        <v>309</v>
+      </c>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="30"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21" s="35" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="E22" s="36"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="28" t="s">
+        <v>308</v>
+      </c>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="30"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="14" t="s">
+        <v>345</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="E24" s="35" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="14" t="s">
+        <v>346</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>232</v>
+      </c>
+      <c r="E25" s="33"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="14" t="s">
+        <v>347</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>233</v>
+      </c>
+      <c r="E26" s="33"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="14" t="s">
+        <v>348</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>234</v>
+      </c>
+      <c r="E27" s="36"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="28" t="s">
+        <v>303</v>
+      </c>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="30"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>272</v>
+      </c>
+      <c r="E29" s="35" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="E30" s="33"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>274</v>
+      </c>
+      <c r="E31" s="33"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="11" t="s">
+        <v>271</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>275</v>
+      </c>
+      <c r="E32" s="33"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E33" s="36"/>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="28" t="s">
+        <v>304</v>
+      </c>
+      <c r="B34" s="29"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="30"/>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="23" t="s">
+        <v>277</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>276</v>
+      </c>
+      <c r="C35" s="7"/>
+      <c r="E35" s="35" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>272</v>
+      </c>
+      <c r="E36" s="33"/>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="E37" s="33"/>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="11" t="s">
+        <v>271</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>275</v>
+      </c>
+      <c r="E38" s="33"/>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="11" t="s">
+        <v>279</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>278</v>
+      </c>
+      <c r="E39" s="33"/>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E40" s="36"/>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="31" t="s">
+        <v>305</v>
+      </c>
+      <c r="B41" s="32"/>
+      <c r="C41" s="32"/>
+      <c r="D41" s="32"/>
+      <c r="E41" s="39"/>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="23" t="s">
+        <v>281</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="C42" s="7"/>
+      <c r="E42" s="35" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="11" t="s">
+        <v>282</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>272</v>
+      </c>
+      <c r="E43" s="33"/>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="11" t="s">
+        <v>283</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="E44" s="33"/>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="11" t="s">
+        <v>284</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>275</v>
+      </c>
+      <c r="E45" s="33"/>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B46" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="E46" s="33"/>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E47" s="36"/>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="28" t="s">
+        <v>306</v>
+      </c>
+      <c r="B48" s="29"/>
+      <c r="C48" s="29"/>
+      <c r="D48" s="29"/>
+      <c r="E48" s="30"/>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="23" t="s">
+        <v>286</v>
+      </c>
+      <c r="B49" s="11" t="s">
+        <v>285</v>
+      </c>
+      <c r="C49" s="7"/>
+      <c r="E49" s="35" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="11" t="s">
+        <v>288</v>
+      </c>
+      <c r="B50" s="11" t="s">
+        <v>287</v>
+      </c>
+      <c r="E50" s="33"/>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="11" t="s">
+        <v>289</v>
+      </c>
+      <c r="B51" s="11" t="s">
+        <v>290</v>
+      </c>
+      <c r="E51" s="33"/>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="11" t="s">
+        <v>292</v>
+      </c>
+      <c r="B52" s="11" t="s">
+        <v>291</v>
+      </c>
+      <c r="E52" s="33"/>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="11" t="s">
+        <v>293</v>
+      </c>
+      <c r="B53" s="11" t="s">
+        <v>294</v>
+      </c>
+      <c r="E53" s="33"/>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="B54" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="C54" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E54" s="36"/>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="28" t="s">
+        <v>307</v>
+      </c>
+      <c r="B55" s="29"/>
+      <c r="C55" s="29"/>
+      <c r="D55" s="29"/>
+      <c r="E55" s="30"/>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="23" t="s">
+        <v>296</v>
+      </c>
+      <c r="B56" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="C56" s="7"/>
+      <c r="D56" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="E56" s="35" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="11" t="s">
+        <v>323</v>
+      </c>
+      <c r="B57" s="11" t="s">
+        <v>297</v>
+      </c>
+      <c r="E57" s="33"/>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="11" t="s">
+        <v>322</v>
+      </c>
+      <c r="B58" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="C58" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="E58" s="33"/>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="B59" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="C59" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E59" s="33"/>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="B60" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="C60" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E60" s="33"/>
+    </row>
+  </sheetData>
+  <mergeCells count="17">
+    <mergeCell ref="E42:E47"/>
+    <mergeCell ref="E49:E54"/>
+    <mergeCell ref="E56:E60"/>
+    <mergeCell ref="E2:E12"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="E14:E19"/>
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="E24:E27"/>
+    <mergeCell ref="A34:E34"/>
+    <mergeCell ref="E29:E33"/>
+    <mergeCell ref="A41:E41"/>
+    <mergeCell ref="E35:E40"/>
+    <mergeCell ref="A48:E48"/>
+    <mergeCell ref="A55:E55"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="E21:E22" r:id="rId1" display="ConfirmDelete.png" xr:uid="{E7D51FE5-38A8-ED48-AB1B-5439A79F0F01}"/>
+    <hyperlink ref="E24:E27" r:id="rId2" display="TaskListMenu.png" xr:uid="{41B9DE7C-F513-7A4C-9608-80B8C1A2E0C8}"/>
+    <hyperlink ref="E2:E12" r:id="rId3" display="TaskList1.png" xr:uid="{BEBE0A19-2F55-7C45-BAFA-8F1ED57A8EB4}"/>
+    <hyperlink ref="E14:E19" r:id="rId4" display="QuickAdd.png" xr:uid="{CC8D6B58-F8B3-F44F-A2A2-CA54AEABDA08}"/>
+    <hyperlink ref="E29:E33" r:id="rId5" display="TasksDue.png" xr:uid="{FFDED12F-6E60-764B-AC50-E9A151FE766C}"/>
+    <hyperlink ref="E35:E40" r:id="rId6" display="TasksStarting.png" xr:uid="{D4E49EAD-B8B9-0A49-B1A0-60F7A38DE2EA}"/>
+    <hyperlink ref="E42:E47" r:id="rId7" display="TasksPriority.png" xr:uid="{ABDF668C-400D-2A4E-86EB-E9FD7C44BF55}"/>
+    <hyperlink ref="E49:E54" r:id="rId8" display="TaskProgress.png" xr:uid="{DF68C727-EFA0-7542-B392-52D12BE8F88E}"/>
+    <hyperlink ref="E56:E60" r:id="rId9" display="Search.png" xr:uid="{226D5616-AE1A-D140-B96F-B62F1F00654E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29DC9B6B-62E5-7B4A-80EC-6F20A2BF6C35}">
+  <dimension ref="A1:E63"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
+  <cols>
+    <col min="1" max="1" width="31" style="11" customWidth="1"/>
+    <col min="2" max="2" width="78" style="11" customWidth="1"/>
+    <col min="3" max="3" width="21.83203125" style="11" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" style="11" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" style="42" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="22" customHeight="1">
+      <c r="A1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" s="43" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="44"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="11" t="s">
+        <v>329</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4" s="44"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="E5" s="37" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="E6" s="33" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="11" t="s">
+        <v>312</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E7" s="33"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="22" t="s">
+        <v>331</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="E8" s="33" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="22" t="s">
+        <v>332</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="E9" s="33"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="22" t="s">
+        <v>293</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="E10" s="33"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="22" t="s">
+        <v>333</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="E11" s="33"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="E12" s="33" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="E13" s="33"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="E14" s="33"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="E15" s="33"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="E16" s="33"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="E17" s="33"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="E18" s="33"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="E19" s="33"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="E20" s="33"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="E21" s="33"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="E22" s="33"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="E23" s="33" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="11" t="s">
+        <v>327</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="E24" s="33"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="E25" s="33"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="E26" s="33"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="E27" s="33"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="B28" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="E28" s="33"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="11" t="s">
+        <v>325</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="E29" s="33"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="22" t="s">
+        <v>335</v>
+      </c>
+      <c r="B30" s="24" t="s">
+        <v>184</v>
+      </c>
+      <c r="E30" s="38"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="22" t="s">
+        <v>336</v>
+      </c>
+      <c r="B31" s="24" t="s">
+        <v>185</v>
+      </c>
+      <c r="E31" s="38"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="22" t="s">
+        <v>337</v>
+      </c>
+      <c r="B32" s="24" t="s">
+        <v>186</v>
+      </c>
+      <c r="E32" s="38"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="22" t="s">
+        <v>338</v>
+      </c>
+      <c r="B33" s="24" t="s">
+        <v>187</v>
+      </c>
+      <c r="E33" s="38"/>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="11" t="s">
+        <v>326</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="E34" s="37" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="22" t="s">
+        <v>339</v>
+      </c>
+      <c r="B35" s="24" t="s">
+        <v>195</v>
+      </c>
+      <c r="E35" s="38"/>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="22" t="s">
+        <v>340</v>
+      </c>
+      <c r="B36" s="24" t="s">
+        <v>194</v>
+      </c>
+      <c r="E36" s="38"/>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="22" t="s">
+        <v>341</v>
+      </c>
+      <c r="B37" s="24" t="s">
+        <v>193</v>
+      </c>
+      <c r="E37" s="38"/>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="22" t="s">
+        <v>342</v>
+      </c>
+      <c r="B38" s="24" t="s">
+        <v>192</v>
+      </c>
+      <c r="E38" s="38"/>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="E39" s="37" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="28" t="s">
+        <v>300</v>
+      </c>
+      <c r="B40" s="29"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="29"/>
+      <c r="E40" s="30"/>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C41" s="15"/>
+      <c r="E41" s="35" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C42" s="15"/>
+      <c r="E42" s="33"/>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="11" t="s">
+        <v>350</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="C43" s="15"/>
+      <c r="E43" s="33"/>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="11" t="s">
+        <v>351</v>
+      </c>
+      <c r="B44" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="C44" s="15"/>
+      <c r="E44" s="33"/>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="11" t="s">
+        <v>352</v>
+      </c>
+      <c r="B45" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="C45" s="15"/>
+      <c r="E45" s="33"/>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="11" t="s">
+        <v>353</v>
+      </c>
+      <c r="B46" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="C46" s="15"/>
+      <c r="E46" s="33"/>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="11" t="s">
+        <v>354</v>
+      </c>
+      <c r="B47" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="C47" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="E47" s="33"/>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="11" t="s">
+        <v>355</v>
+      </c>
+      <c r="B48" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="C48" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="E48" s="37" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="28" t="s">
+        <v>301</v>
+      </c>
+      <c r="B49" s="29"/>
+      <c r="C49" s="29"/>
+      <c r="D49" s="29"/>
+      <c r="E49" s="30"/>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="B50" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C50" s="15"/>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="B51" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C51" s="15"/>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="B52" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="C52" s="15"/>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="B53" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="C53" s="15"/>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="B54" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="C54" s="15"/>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B55" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="C55" s="15" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="B56" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="C56" s="15" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="B57" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="C57" s="15"/>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B58" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="C58" s="15"/>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="B59" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="C59" s="15"/>
+      <c r="D59" s="11" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="B60" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="C60" s="15"/>
+      <c r="D60" s="11" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="B61" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="C61" s="15"/>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="22" t="s">
+        <v>343</v>
+      </c>
+      <c r="B62" s="24" t="s">
+        <v>169</v>
+      </c>
+      <c r="C62" s="15"/>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="22" t="s">
+        <v>344</v>
+      </c>
+      <c r="B63" s="24" t="s">
+        <v>170</v>
+      </c>
+      <c r="C63" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="E8:E11"/>
+    <mergeCell ref="E30:E33"/>
+    <mergeCell ref="E35:E38"/>
+    <mergeCell ref="A40:E40"/>
+    <mergeCell ref="A49:E49"/>
+    <mergeCell ref="E12:E22"/>
+    <mergeCell ref="E23:E29"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="E41:E47"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="E12:E22" r:id="rId1" display="EditTask1.png" xr:uid="{9FE2AE8E-A9CA-964E-A11C-56069919D277}"/>
+    <hyperlink ref="E2:E4" r:id="rId2" display="EditTask1.png" xr:uid="{AF945763-504F-F44B-941F-F68473F43173}"/>
+    <hyperlink ref="E5" r:id="rId3" xr:uid="{C90C6E02-C85B-3048-B0C9-FEDCC070B8E1}"/>
+    <hyperlink ref="E6:E7" r:id="rId4" display="EditTask1.png" xr:uid="{7200B3E4-19A9-E34E-B217-AC9A8F0454BD}"/>
+    <hyperlink ref="E8:E11" r:id="rId5" display="StatusOptions.png" xr:uid="{57BBB0F1-C4D2-0645-BB6D-452C7CF30353}"/>
+    <hyperlink ref="E23:E29" r:id="rId6" display="EditTask2.png" xr:uid="{1B62641F-1A9C-CA4B-B9EA-354F0B02D7F0}"/>
+    <hyperlink ref="E34" r:id="rId7" xr:uid="{8446D4E4-077D-0A4D-8525-8FB07FF0C373}"/>
+    <hyperlink ref="E39" r:id="rId8" xr:uid="{12FBB57A-780E-814C-87D8-AFBFE84831F1}"/>
+    <hyperlink ref="E41:E47" r:id="rId9" display="Calendar.png" xr:uid="{610945C3-6CA0-044C-8FF8-83DD72D73D6A}"/>
+    <hyperlink ref="E48" r:id="rId10" xr:uid="{7E1BB3A1-2AEF-CA43-9C3D-463F6622F876}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{103321A1-C480-514F-9128-290C60DCE81A}">
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
+  <cols>
+    <col min="1" max="1" width="24.83203125" style="20" customWidth="1"/>
+    <col min="2" max="2" width="118.6640625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" style="11" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" style="11" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="20" t="s">
+        <v>200</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="20" t="s">
+        <v>201</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="20" t="s">
+        <v>302</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="21" t="s">
+        <v>224</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="21" t="s">
+        <v>228</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="20" t="s">
+        <v>208</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="20" t="s">
+        <v>212</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="20" t="s">
+        <v>215</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="20" t="s">
+        <v>218</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="25" t="s">
+        <v>309</v>
+      </c>
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="27"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53604592-2150-C948-A745-A2773E7BE451}">
+  <dimension ref="A1:D23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
+  <cols>
+    <col min="1" max="1" width="27.6640625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="113.6640625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" style="11" customWidth="1"/>
+    <col min="4" max="4" width="14" style="11" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="11" t="s">
+        <v>265</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="28" t="s">
+        <v>310</v>
+      </c>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="30"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="11" t="s">
+        <v>263</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="28" t="s">
+        <v>311</v>
+      </c>
+      <c r="B17" s="29"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="30"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="11" t="s">
+        <v>256</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="11" t="s">
+        <v>258</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>255</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A17:D17"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{296F9A35-BE5A-E64F-9080-864E7183DD30}">
   <dimension ref="A1:K83"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -2973,1617 +4961,4 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EF6FCC3-78DA-E74D-BF53-4A0FCE774DC3}">
-  <dimension ref="A1:D60"/>
-  <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
-  <cols>
-    <col min="1" max="1" width="31" style="11" customWidth="1"/>
-    <col min="2" max="2" width="99.33203125" style="11" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" style="11" customWidth="1"/>
-    <col min="4" max="4" width="16.5" style="11" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="11"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="21" customHeight="1">
-      <c r="A1" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="C5" s="12"/>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6" s="12"/>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="C7" s="12"/>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="C8" s="12"/>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="11" t="s">
-        <v>304</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="C9" s="12"/>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="28" t="s">
-        <v>300</v>
-      </c>
-      <c r="B13" s="29"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="30"/>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>196</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="28" t="s">
-        <v>315</v>
-      </c>
-      <c r="B20" s="29"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="30"/>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="11" t="s">
-        <v>226</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="28" t="s">
-        <v>310</v>
-      </c>
-      <c r="B23" s="29"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="30"/>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="14" t="s">
-        <v>311</v>
-      </c>
-      <c r="B24" s="14" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="14" t="s">
-        <v>312</v>
-      </c>
-      <c r="B25" s="14" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="14" t="s">
-        <v>313</v>
-      </c>
-      <c r="B26" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="14" t="s">
-        <v>314</v>
-      </c>
-      <c r="B27" s="14" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="28" t="s">
-        <v>305</v>
-      </c>
-      <c r="B28" s="29"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="30"/>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="11" t="s">
-        <v>268</v>
-      </c>
-      <c r="B29" s="11" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="11" t="s">
-        <v>270</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="11" t="s">
-        <v>271</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="B33" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="28" t="s">
-        <v>306</v>
-      </c>
-      <c r="B34" s="29"/>
-      <c r="C34" s="29"/>
-      <c r="D34" s="30"/>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="23" t="s">
-        <v>277</v>
-      </c>
-      <c r="B35" s="11" t="s">
-        <v>276</v>
-      </c>
-      <c r="C35" s="7"/>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="11" t="s">
-        <v>268</v>
-      </c>
-      <c r="B36" s="11" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="B37" s="11" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="11" t="s">
-        <v>271</v>
-      </c>
-      <c r="B38" s="11" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="11" t="s">
-        <v>279</v>
-      </c>
-      <c r="B39" s="11" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="B40" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="C40" s="12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="28" t="s">
-        <v>307</v>
-      </c>
-      <c r="B41" s="29"/>
-      <c r="C41" s="29"/>
-      <c r="D41" s="30"/>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="23" t="s">
-        <v>281</v>
-      </c>
-      <c r="B42" s="11" t="s">
-        <v>280</v>
-      </c>
-      <c r="C42" s="7"/>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="11" t="s">
-        <v>282</v>
-      </c>
-      <c r="B43" s="11" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="11" t="s">
-        <v>283</v>
-      </c>
-      <c r="B44" s="11" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="11" t="s">
-        <v>284</v>
-      </c>
-      <c r="B45" s="11" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B46" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="C46" s="14" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="B47" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="C47" s="12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="28" t="s">
-        <v>308</v>
-      </c>
-      <c r="B48" s="29"/>
-      <c r="C48" s="29"/>
-      <c r="D48" s="30"/>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="23" t="s">
-        <v>286</v>
-      </c>
-      <c r="B49" s="11" t="s">
-        <v>285</v>
-      </c>
-      <c r="C49" s="7"/>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="A50" s="11" t="s">
-        <v>288</v>
-      </c>
-      <c r="B50" s="11" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="11" t="s">
-        <v>289</v>
-      </c>
-      <c r="B51" s="11" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" s="11" t="s">
-        <v>292</v>
-      </c>
-      <c r="B52" s="11" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="11" t="s">
-        <v>293</v>
-      </c>
-      <c r="B53" s="11" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="B54" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="C54" s="12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="28" t="s">
-        <v>309</v>
-      </c>
-      <c r="B55" s="29"/>
-      <c r="C55" s="29"/>
-      <c r="D55" s="30"/>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="23" t="s">
-        <v>296</v>
-      </c>
-      <c r="B56" s="11" t="s">
-        <v>295</v>
-      </c>
-      <c r="C56" s="7"/>
-      <c r="D56" s="11" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="11" t="s">
-        <v>297</v>
-      </c>
-      <c r="B57" s="11" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="11" t="s">
-        <v>299</v>
-      </c>
-      <c r="B58" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="C58" s="14" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="A59" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="B59" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="C59" s="12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
-      <c r="A60" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="B60" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="C60" s="12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A55:D55"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="A41:D41"/>
-    <mergeCell ref="A48:D48"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29DC9B6B-62E5-7B4A-80EC-6F20A2BF6C35}">
-  <dimension ref="A1:D63"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
-  <cols>
-    <col min="1" max="1" width="31" style="11" customWidth="1"/>
-    <col min="2" max="2" width="78" style="11" customWidth="1"/>
-    <col min="3" max="3" width="21.83203125" style="11" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" style="11" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="11"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="22" customHeight="1">
-      <c r="A1" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>196</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>150</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="22" t="s">
-        <v>172</v>
-      </c>
-      <c r="B28" s="24" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="11" t="s">
-        <v>180</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="11" t="s">
-        <v>181</v>
-      </c>
-      <c r="B31" s="15" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="B32" s="15" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="B33" s="15" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="B34" s="15" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="B35" s="15" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="B36" s="15" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="11" t="s">
-        <v>190</v>
-      </c>
-      <c r="B37" s="15" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="11" t="s">
-        <v>191</v>
-      </c>
-      <c r="B38" s="15" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="B39" s="15" t="s">
-        <v>178</v>
-      </c>
-      <c r="D39" s="11" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="28" t="s">
-        <v>302</v>
-      </c>
-      <c r="B40" s="29"/>
-      <c r="C40" s="29"/>
-      <c r="D40" s="30"/>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="B41" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="C41" s="15"/>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="B42" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="C42" s="15"/>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="B43" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="C43" s="15"/>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="B44" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="C44" s="15"/>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="B45" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="C45" s="15"/>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="B46" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="C46" s="15"/>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="B47" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="C47" s="15" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="B48" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="C48" s="15" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="28" t="s">
-        <v>303</v>
-      </c>
-      <c r="B49" s="29"/>
-      <c r="C49" s="29"/>
-      <c r="D49" s="30"/>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="A50" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="B50" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="C50" s="15"/>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="B51" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="C51" s="15"/>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="B52" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="C52" s="15"/>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="B53" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="C53" s="15"/>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="B54" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="C54" s="15"/>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="B55" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="C55" s="15" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="B56" s="15" t="s">
-        <v>158</v>
-      </c>
-      <c r="C56" s="15" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="B57" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="C57" s="15"/>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="B58" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="C58" s="15"/>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="A59" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="B59" s="15" t="s">
-        <v>163</v>
-      </c>
-      <c r="C59" s="15"/>
-      <c r="D59" s="11" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
-      <c r="A60" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="B60" s="15" t="s">
-        <v>164</v>
-      </c>
-      <c r="C60" s="15"/>
-      <c r="D60" s="11" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
-      <c r="A61" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="B61" s="15" t="s">
-        <v>166</v>
-      </c>
-      <c r="C61" s="15"/>
-    </row>
-    <row r="62" spans="1:4">
-      <c r="A62" s="11" t="s">
-        <v>167</v>
-      </c>
-      <c r="B62" s="15" t="s">
-        <v>169</v>
-      </c>
-      <c r="C62" s="15"/>
-    </row>
-    <row r="63" spans="1:4">
-      <c r="A63" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="B63" s="15" t="s">
-        <v>170</v>
-      </c>
-      <c r="C63" s="15"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A40:D40"/>
-    <mergeCell ref="A49:D49"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{103321A1-C480-514F-9128-290C60DCE81A}">
-  <dimension ref="A1:D22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
-  <cols>
-    <col min="1" max="1" width="24.83203125" style="20" customWidth="1"/>
-    <col min="2" max="2" width="118.6640625" style="11" customWidth="1"/>
-    <col min="3" max="3" width="26.6640625" style="11" customWidth="1"/>
-    <col min="4" max="4" width="18.83203125" style="11" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="11"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="20" t="s">
-        <v>200</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="20" t="s">
-        <v>201</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="20" t="s">
-        <v>203</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="20" t="s">
-        <v>304</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="21" t="s">
-        <v>222</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="21" t="s">
-        <v>224</v>
-      </c>
-      <c r="B7" s="22" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="21" t="s">
-        <v>228</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="21" t="s">
-        <v>230</v>
-      </c>
-      <c r="B9" s="22" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="20" t="s">
-        <v>205</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="20" t="s">
-        <v>206</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="20" t="s">
-        <v>208</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="20" t="s">
-        <v>212</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>238</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>239</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="20" t="s">
-        <v>214</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>240</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="20" t="s">
-        <v>215</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="20" t="s">
-        <v>218</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="20" t="s">
-        <v>220</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="25" t="s">
-        <v>315</v>
-      </c>
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="27"/>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="11" t="s">
-        <v>226</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>74</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53604592-2150-C948-A745-A2773E7BE451}">
-  <dimension ref="A1:D23"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
-  <cols>
-    <col min="1" max="1" width="27.6640625" style="11" customWidth="1"/>
-    <col min="2" max="2" width="113.6640625" style="11" customWidth="1"/>
-    <col min="3" max="3" width="23.33203125" style="11" customWidth="1"/>
-    <col min="4" max="4" width="14" style="11" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="11"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="11" t="s">
-        <v>200</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="11" t="s">
-        <v>235</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>237</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="11" t="s">
-        <v>241</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>242</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="11" t="s">
-        <v>244</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="11" t="s">
-        <v>264</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="11" t="s">
-        <v>265</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="28" t="s">
-        <v>316</v>
-      </c>
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="30"/>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="11" t="s">
-        <v>245</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="11" t="s">
-        <v>226</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="11" t="s">
-        <v>248</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="11" t="s">
-        <v>249</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="11" t="s">
-        <v>250</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="11" t="s">
-        <v>263</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="28" t="s">
-        <v>317</v>
-      </c>
-      <c r="B17" s="29"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="30"/>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="11" t="s">
-        <v>261</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>262</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="11" t="s">
-        <v>256</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="11" t="s">
-        <v>258</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="11" t="s">
-        <v>259</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="11" t="s">
-        <v>260</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>255</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A17:D17"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>